<commit_message>
* Update key dates page to be chronologically sorted
</commit_message>
<xml_diff>
--- a/data/key_dates.xlsx
+++ b/data/key_dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://idorsia-my.sharepoint.com/personal/joana_marques-barros_idorsia_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\widmelu1\Downloads\iscb2025-site\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71D70502-8290-455C-9F41-AEBC8D90EDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7058F45-5873-42D6-9BA7-4BED124EC274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8EAE64F2-7715-4A3F-9B05-9B8368B4BEE5}"/>
+    <workbookView xWindow="13830" yWindow="2610" windowWidth="24165" windowHeight="14160" xr2:uid="{8EAE64F2-7715-4A3F-9B05-9B8368B4BEE5}"/>
   </bookViews>
   <sheets>
     <sheet name="ISCB" sheetId="7" r:id="rId1"/>
@@ -39,71 +39,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Awards application</t>
   </si>
   <si>
-    <t>Invited sessions</t>
-  </si>
-  <si>
     <t>Call</t>
   </si>
   <si>
     <t>Notifications sent</t>
   </si>
   <si>
-    <t>Topic-contributed sessions</t>
-  </si>
-  <si>
     <t>Short courses</t>
   </si>
   <si>
     <t>Abstracts</t>
   </si>
   <si>
-    <t>Posters</t>
-  </si>
-  <si>
     <t xml:space="preserve">Registration </t>
   </si>
   <si>
     <t>Sunday, 24 August 2025</t>
   </si>
   <si>
-    <t>Monday, 24 February 2025</t>
-  </si>
-  <si>
-    <t>Monday, 22 July 2024</t>
-  </si>
-  <si>
-    <t>Monday, 21 October 2024</t>
-  </si>
-  <si>
-    <t>Thursday, 7 November 2024</t>
-  </si>
-  <si>
-    <t>Saturday, 5 October 2024</t>
-  </si>
-  <si>
     <t>Sunday, 5 January 2025</t>
   </si>
   <si>
-    <t>Wednesday, 5 February 2025</t>
-  </si>
-  <si>
-    <t>Thursday, 21 November 2024</t>
-  </si>
-  <si>
     <t>Sunday, 23 February 2025</t>
   </si>
   <si>
     <t>Friday, 21 March 2025</t>
   </si>
   <si>
-    <t>Saturday, 22 March 2025</t>
-  </si>
-  <si>
     <t>Wednesday, 21 May 2025</t>
   </si>
   <si>
@@ -147,6 +114,27 @@
   </si>
   <si>
     <t>Thursday, 28 August 2025</t>
+  </si>
+  <si>
+    <t>Friday, 8 November 2024</t>
+  </si>
+  <si>
+    <t>Sunday, 20 October 2024</t>
+  </si>
+  <si>
+    <t>Friday, 4 October 2024</t>
+  </si>
+  <si>
+    <t>Friday, 7 February 2025</t>
+  </si>
+  <si>
+    <t>Monday, 29 July 2024</t>
+  </si>
+  <si>
+    <t>Friday, 22 November 2024</t>
+  </si>
+  <si>
+    <t>Contributed sessions</t>
   </si>
 </sst>
 </file>
@@ -154,7 +142,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -206,15 +194,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,46 +537,46 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -604,73 +589,72 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.77734375" customWidth="1"/>
-    <col min="2" max="5" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -679,198 +663,143 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE1B740-4E63-4388-94FB-88B4A58C9FD2}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B24" s="5"/>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -882,40 +811,40 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H37" s="5"/>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update: abstract submission deadline
</commit_message>
<xml_diff>
--- a/data/key_dates.xlsx
+++ b/data/key_dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marqujo1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFE00F8-B858-42F6-AFC6-D6C25CC5EA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0645A17D-EB17-45EC-8102-AEB2AB773A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10850" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{8EAE64F2-7715-4A3F-9B05-9B8368B4BEE5}"/>
+    <workbookView xWindow="19940" yWindow="-510" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{8EAE64F2-7715-4A3F-9B05-9B8368B4BEE5}"/>
   </bookViews>
   <sheets>
     <sheet name="ISCB" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>Awards application</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Thursday, 07 November 2024</t>
+  </si>
+  <si>
+    <t>Friday, 14 February 2025</t>
   </si>
 </sst>
 </file>
@@ -666,7 +669,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,7 +742,7 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add: non-extendable note to abstract submission deadline
</commit_message>
<xml_diff>
--- a/data/key_dates.xlsx
+++ b/data/key_dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marqujo1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0645A17D-EB17-45EC-8102-AEB2AB773A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3BA079-0427-4F7A-9089-3B8FF89D1366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19940" yWindow="-510" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{8EAE64F2-7715-4A3F-9B05-9B8368B4BEE5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{8EAE64F2-7715-4A3F-9B05-9B8368B4BEE5}"/>
   </bookViews>
   <sheets>
     <sheet name="ISCB" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>Awards application</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Friday, 14 February 2025</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>(non-extendable)</t>
   </si>
 </sst>
 </file>
@@ -666,10 +672,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE1B740-4E63-4388-94FB-88B4A58C9FD2}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,9 +683,10 @@
     <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -689,8 +696,11 @@
       <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -701,7 +711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -712,7 +722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -723,7 +733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -734,7 +744,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -744,8 +754,11 @@
       <c r="C6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -756,7 +769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -767,7 +780,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -778,7 +791,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -789,19 +802,19 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tidy key-dates files. Keep original structure and just rename contributed sessions to invited sessions
</commit_message>
<xml_diff>
--- a/data/key_dates.xlsx
+++ b/data/key_dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marqujo1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3BA079-0427-4F7A-9089-3B8FF89D1366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE557BED-304E-4317-82CF-8B3BC74FE9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{8EAE64F2-7715-4A3F-9B05-9B8368B4BEE5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8EAE64F2-7715-4A3F-9B05-9B8368B4BEE5}"/>
   </bookViews>
   <sheets>
     <sheet name="ISCB" sheetId="7" r:id="rId1"/>
@@ -128,22 +128,22 @@
     <t>Invited Sessions</t>
   </si>
   <si>
-    <t>Monday, 22 July 2024</t>
-  </si>
-  <si>
-    <t>Monday, 21 October 2024</t>
-  </si>
-  <si>
-    <t>Thursday, 07 November 2024</t>
-  </si>
-  <si>
     <t>Friday, 14 February 2025</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>(non-extendable)</t>
+    <t>Non-extendable</t>
+  </si>
+  <si>
+    <t>Monday, 29 July 2024</t>
+  </si>
+  <si>
+    <t>Sunday, 20 October 2024</t>
+  </si>
+  <si>
+    <t>Friday, 8 November 2024</t>
   </si>
 </sst>
 </file>
@@ -203,12 +203,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,13 +550,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -566,7 +567,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -577,7 +578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -601,13 +602,13 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="5" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -618,7 +619,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -629,7 +630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -640,7 +641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -651,7 +652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -662,7 +663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
     </row>
   </sheetData>
@@ -675,18 +676,18 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -697,124 +698,124 @@
         <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
     </row>
   </sheetData>
@@ -830,14 +831,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -848,7 +849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -859,7 +860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H37" s="4"/>
     </row>
   </sheetData>

</xml_diff>